<commit_message>
added report and other stuff
</commit_message>
<xml_diff>
--- a/Phase3/plot.xlsx
+++ b/Phase3/plot.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="41">
   <si>
     <t>Run</t>
   </si>
@@ -34,20 +34,63 @@
     <t>4</t>
   </si>
   <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2
+    <t>0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1818181818181818181818181818
 </t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>0.1666666666666666666666666667</t>
+    <t>0.3333333333333333333333333333</t>
   </si>
   <si>
     <t>33</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09090909090909090909090909091
+</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2727272727272727272727272727
+</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>tfidf_stop</t>
+  </si>
+  <si>
+    <t>0.3636363636363636363636363636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3636363636363636363636363636
+</t>
+  </si>
+  <si>
+    <t>0.4285714285714285714285714286</t>
+  </si>
+  <si>
+    <t>bm25</t>
+  </si>
+  <si>
+    <t>0.7142857142857142857142857143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4545454545454545454545454545
+</t>
   </si>
   <si>
     <t>0</t>
@@ -57,85 +100,50 @@
 </t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6
+    <t>0.2941176470588235294117647059</t>
+  </si>
+  <si>
+    <t>jm</t>
+  </si>
+  <si>
+    <t>0.8333333333333333333333333333</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>jm_stop</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>bm_queryEnrichment</t>
+  </si>
+  <si>
+    <t>0.6666666666666666666666666667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5454545454545454545454545455
 </t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>0.3333333333333333333333333333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4
-</t>
-  </si>
-  <si>
-    <t>tfidf_stop</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.2727272727272727272727272727</t>
-  </si>
-  <si>
-    <t>0.2857142857142857142857142857</t>
-  </si>
-  <si>
-    <t>bm25</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.5714285714285714285714285714</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8
-</t>
-  </si>
-  <si>
-    <t>0.1176470588235294117647058824</t>
-  </si>
-  <si>
-    <t>jm</t>
-  </si>
-  <si>
-    <t>0.6666666666666666666666666667</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>jm_stop</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>0.125</t>
-  </si>
-  <si>
-    <t>bm_queryEnrichment</t>
-  </si>
-  <si>
-    <t>0.1111111111111111111111111111</t>
-  </si>
-  <si>
     <t>bm_stop</t>
   </si>
   <si>
+    <t>0.3125</t>
+  </si>
+  <si>
     <t>lucene</t>
   </si>
   <si>
-    <t>0.4285714285714285714285714286</t>
+    <t>0.1764705882352941176470588235</t>
   </si>
 </sst>
 </file>
@@ -560,15 +568,15 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -582,69 +590,69 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -652,69 +660,69 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -722,55 +730,55 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -778,69 +786,69 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -854,10 +862,10 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -868,10 +876,10 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -882,10 +890,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -896,10 +904,10 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -910,7 +918,7 @@
         <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -918,139 +926,139 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
         <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>

</xml_diff>